<commit_message>
Add first test for rules builder class
</commit_message>
<xml_diff>
--- a/dummy-rules.xlsx
+++ b/dummy-rules.xlsx
@@ -12,15 +12,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>Score</t>
+  </si>
   <si>
     <t>Your time is up, old timer</t>
   </si>
   <si>
-    <t>Score</t>
+    <t>Rule</t>
   </si>
   <si>
-    <t>Rule</t>
+    <t>Senior citizens don't belong in the ring</t>
   </si>
 </sst>
 </file>
@@ -33,10 +36,10 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
       <b/>
     </font>
+    <font/>
     <font>
       <u/>
       <color rgb="FF0000FF"/>
@@ -66,7 +69,7 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -97,15 +100,15 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="6.29"/>
-    <col customWidth="1" min="2" max="2" width="16.43"/>
+    <col customWidth="1" min="2" max="2" width="17.86"/>
     <col customWidth="1" min="3" max="3" width="23.29"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
-        <v>1</v>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3"/>
@@ -133,7 +136,7 @@
       <c r="Z1" s="3"/>
     </row>
     <row r="2">
-      <c r="A2" s="1">
+      <c r="A2" s="2">
         <v>1.0</v>
       </c>
       <c r="B2" s="4" t="str">
@@ -156,12 +159,17 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="21.57"/>
+    <col customWidth="1" min="1" max="1" width="32.43"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>